<commit_message>
add fleet level analyis
</commit_message>
<xml_diff>
--- a/test_env/database_creation/rawdata/aircraftproperties/Aircraft Databank v2.xlsx
+++ b/test_env/database_creation/rawdata/aircraftproperties/Aircraft Databank v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRohr\Desktop\Masterarbeit\Python\test_env\database_creation\rawdata\aircraftproperties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0BAC2B-1E6D-407B-BD00-5CBC076ACB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D70971-5126-426B-AC51-C01D414A897F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="1" activeTab="1" xr2:uid="{B2B150D8-E64E-4875-9280-D2B2D82F52FA}"/>
+    <workbookView xWindow="-90" yWindow="-21600" windowWidth="24550" windowHeight="20970" firstSheet="1" activeTab="1" xr2:uid="{B2B150D8-E64E-4875-9280-D2B2D82F52FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Table" sheetId="1" r:id="rId1"/>
@@ -3655,9 +3655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7E994-12F2-4962-AF8C-42BF75C864FA}">
   <dimension ref="A1:P189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A190" sqref="A190:XFD190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>

</xml_diff>